<commit_message>
premysleni o strukture DB
</commit_message>
<xml_diff>
--- a/PDMSCore/wwwroot/TestDB/StrukturaDB.xlsx
+++ b/PDMSCore/wwwroot/TestDB/StrukturaDB.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="196">
   <si>
     <t>Technicke jmeno</t>
   </si>
@@ -600,12 +601,117 @@
   <si>
     <t>MultiSelection</t>
   </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>RetailersProjects</t>
+  </si>
+  <si>
+    <t>RetailersPage</t>
+  </si>
+  <si>
+    <t>Ahoj</t>
+  </si>
+  <si>
+    <t>Zdar</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>FieldVal</t>
+  </si>
+  <si>
+    <t>NeAhoj</t>
+  </si>
+  <si>
+    <t>NeZdar</t>
+  </si>
+  <si>
+    <t>*a</t>
+  </si>
+  <si>
+    <t>*b</t>
+  </si>
+  <si>
+    <t>*c</t>
+  </si>
+  <si>
+    <t>*d</t>
+  </si>
+  <si>
+    <t>*f</t>
+  </si>
+  <si>
+    <t>ProjectFieldVal</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>j4</t>
+  </si>
+  <si>
+    <t>k4</t>
+  </si>
+  <si>
+    <t>l4</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,8 +767,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,8 +849,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -876,11 +1002,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -977,6 +1140,40 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,12 +1189,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1010,28 +1201,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,7 +1542,7 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:D27"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,31 +1566,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
       <c r="D1" s="6"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
+      <c r="F1" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
+      <c r="N1" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1627,17 +1854,17 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="K11" s="73" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="K11" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="73"/>
+      <c r="L11" s="78"/>
       <c r="N11">
         <v>4</v>
       </c>
@@ -1664,11 +1891,11 @@
       <c r="E12" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="70" t="s">
+      <c r="G12" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="71"/>
-      <c r="I12" s="72"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="84"/>
       <c r="K12" s="10" t="s">
         <v>46</v>
       </c>
@@ -1929,12 +2156,12 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="5"/>
       <c r="N21">
         <v>9</v>
@@ -2108,20 +2335,20 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="G30" s="74" t="s">
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="G30" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
       <c r="N30">
         <v>15</v>
       </c>
@@ -2487,17 +2714,17 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="E43" s="73" t="s">
+      <c r="C43" s="79"/>
+      <c r="E43" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="73"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
-      <c r="I43" s="73"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="78"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
@@ -2717,13 +2944,13 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="68" t="s">
+      <c r="A56" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -2879,11 +3106,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="K11:L11"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="A11:E11"/>
@@ -2892,6 +3114,11 @@
     <mergeCell ref="G30:K30"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="B43:C43"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2900,11 +3127,607 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="S20" sqref="S20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H2" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="88"/>
+    </row>
+    <row r="3" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="I3" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="106"/>
+    </row>
+    <row r="4" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="99"/>
+      <c r="M4" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="N4" s="88"/>
+    </row>
+    <row r="5" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K5" s="88" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+    </row>
+    <row r="6" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H6" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="M6" s="108" t="s">
+        <v>123</v>
+      </c>
+      <c r="N6" s="109" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H7" s="97">
+        <v>1</v>
+      </c>
+      <c r="I7" s="93">
+        <v>1</v>
+      </c>
+      <c r="J7" s="93">
+        <v>1</v>
+      </c>
+      <c r="K7" s="112">
+        <v>1</v>
+      </c>
+      <c r="L7" s="92" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" s="102">
+        <v>1</v>
+      </c>
+      <c r="N7" s="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="98"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="112">
+        <v>2</v>
+      </c>
+      <c r="L8" s="92" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" s="103"/>
+      <c r="N8" s="98"/>
+    </row>
+    <row r="9" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H9" s="98"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="97">
+        <v>2</v>
+      </c>
+      <c r="K9" s="90">
+        <v>3</v>
+      </c>
+      <c r="L9" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="M9" s="103"/>
+      <c r="N9" s="98"/>
+    </row>
+    <row r="10" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="98"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="90">
+        <v>4</v>
+      </c>
+      <c r="L10" s="90" t="s">
+        <v>167</v>
+      </c>
+      <c r="M10" s="103"/>
+      <c r="N10" s="98"/>
+    </row>
+    <row r="11" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="98"/>
+      <c r="I11" s="97">
+        <v>2</v>
+      </c>
+      <c r="J11" s="97">
+        <v>3</v>
+      </c>
+      <c r="K11" s="92">
+        <v>5</v>
+      </c>
+      <c r="L11" s="92" t="s">
+        <v>168</v>
+      </c>
+      <c r="M11" s="103"/>
+      <c r="N11" s="98"/>
+    </row>
+    <row r="12" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="90">
+        <v>6</v>
+      </c>
+      <c r="L12" s="90" t="s">
+        <v>169</v>
+      </c>
+      <c r="M12" s="103"/>
+      <c r="N12" s="98"/>
+    </row>
+    <row r="13" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="97">
+        <v>4</v>
+      </c>
+      <c r="K13" s="92">
+        <v>5</v>
+      </c>
+      <c r="L13" s="92" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="103"/>
+      <c r="N13" s="98"/>
+    </row>
+    <row r="14" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="98"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="90">
+        <v>8</v>
+      </c>
+      <c r="L14" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14" s="104"/>
+      <c r="N14" s="98"/>
+    </row>
+    <row r="15" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="98"/>
+      <c r="I15" s="93">
+        <v>1</v>
+      </c>
+      <c r="J15" s="93">
+        <v>1</v>
+      </c>
+      <c r="K15" s="112">
+        <v>1</v>
+      </c>
+      <c r="L15" s="107" t="s">
+        <v>176</v>
+      </c>
+      <c r="M15" s="102">
+        <v>2</v>
+      </c>
+      <c r="N15" s="98"/>
+    </row>
+    <row r="16" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="98"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="112">
+        <v>2</v>
+      </c>
+      <c r="L16" s="101" t="s">
+        <v>177</v>
+      </c>
+      <c r="M16" s="103"/>
+      <c r="N16" s="98"/>
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H17" s="98"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="97">
+        <v>2</v>
+      </c>
+      <c r="K17" s="90">
+        <v>3</v>
+      </c>
+      <c r="L17" s="90" t="s">
+        <v>178</v>
+      </c>
+      <c r="M17" s="103"/>
+      <c r="N17" s="98"/>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H18" s="98"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="90">
+        <v>4</v>
+      </c>
+      <c r="L18" s="90" t="s">
+        <v>179</v>
+      </c>
+      <c r="M18" s="103"/>
+      <c r="N18" s="98"/>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H19" s="98"/>
+      <c r="I19" s="97">
+        <v>2</v>
+      </c>
+      <c r="J19" s="97">
+        <v>3</v>
+      </c>
+      <c r="K19" s="92">
+        <v>5</v>
+      </c>
+      <c r="L19" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="M19" s="103"/>
+      <c r="N19" s="98"/>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="90">
+        <v>6</v>
+      </c>
+      <c r="L20" s="90" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" s="103"/>
+      <c r="N20" s="98"/>
+    </row>
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="97">
+        <v>4</v>
+      </c>
+      <c r="K21" s="92">
+        <v>5</v>
+      </c>
+      <c r="L21" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="M21" s="103"/>
+      <c r="N21" s="98"/>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="90">
+        <v>8</v>
+      </c>
+      <c r="L22" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="M22" s="104"/>
+      <c r="N22" s="96"/>
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H23" s="97">
+        <v>2</v>
+      </c>
+      <c r="I23" s="93">
+        <v>1</v>
+      </c>
+      <c r="J23" s="93">
+        <v>1</v>
+      </c>
+      <c r="K23" s="112">
+        <v>1</v>
+      </c>
+      <c r="L23" s="92" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="102">
+        <v>3</v>
+      </c>
+      <c r="N23" s="97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H24" s="98"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="112">
+        <v>2</v>
+      </c>
+      <c r="L24" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="M24" s="103"/>
+      <c r="N24" s="98"/>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H25" s="98"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="97">
+        <v>2</v>
+      </c>
+      <c r="K25" s="90">
+        <v>11</v>
+      </c>
+      <c r="L25" s="90" t="s">
+        <v>184</v>
+      </c>
+      <c r="M25" s="103"/>
+      <c r="N25" s="98"/>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H26" s="98"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="90">
+        <v>12</v>
+      </c>
+      <c r="L26" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="M26" s="103"/>
+      <c r="N26" s="98"/>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H27" s="98"/>
+      <c r="I27" s="97">
+        <v>3</v>
+      </c>
+      <c r="J27" s="111" t="s">
+        <v>194</v>
+      </c>
+      <c r="K27" s="90">
+        <v>13</v>
+      </c>
+      <c r="L27" s="90" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" s="103"/>
+      <c r="N27" s="98"/>
+    </row>
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="90">
+        <v>14</v>
+      </c>
+      <c r="L28" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="M28" s="103"/>
+      <c r="N28" s="98"/>
+    </row>
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="K29" s="90">
+        <v>15</v>
+      </c>
+      <c r="L29" s="90" t="s">
+        <v>174</v>
+      </c>
+      <c r="M29" s="103"/>
+      <c r="N29" s="98"/>
+    </row>
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H30" s="98"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="90">
+        <v>16</v>
+      </c>
+      <c r="L30" s="90" t="s">
+        <v>185</v>
+      </c>
+      <c r="M30" s="104"/>
+      <c r="N30" s="98"/>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="98"/>
+      <c r="I31" s="93">
+        <v>1</v>
+      </c>
+      <c r="J31" s="93">
+        <v>1</v>
+      </c>
+      <c r="K31" s="112">
+        <v>1</v>
+      </c>
+      <c r="L31" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="M31" s="102">
+        <v>4</v>
+      </c>
+      <c r="N31" s="98"/>
+    </row>
+    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H32" s="98"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="112">
+        <v>2</v>
+      </c>
+      <c r="L32" s="92" t="s">
+        <v>187</v>
+      </c>
+      <c r="M32" s="103"/>
+      <c r="N32" s="98"/>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H33" s="98"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="97">
+        <v>2</v>
+      </c>
+      <c r="K33" s="90">
+        <v>11</v>
+      </c>
+      <c r="L33" s="90" t="s">
+        <v>188</v>
+      </c>
+      <c r="M33" s="103"/>
+      <c r="N33" s="98"/>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H34" s="98"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="90">
+        <v>12</v>
+      </c>
+      <c r="L34" s="90" t="s">
+        <v>189</v>
+      </c>
+      <c r="M34" s="103"/>
+      <c r="N34" s="98"/>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H35" s="98"/>
+      <c r="I35" s="97">
+        <v>3</v>
+      </c>
+      <c r="J35" s="111" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" s="90">
+        <v>13</v>
+      </c>
+      <c r="L35" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="M35" s="103"/>
+      <c r="N35" s="98"/>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="90">
+        <v>14</v>
+      </c>
+      <c r="L36" s="90" t="s">
+        <v>191</v>
+      </c>
+      <c r="M36" s="103"/>
+      <c r="N36" s="98"/>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H37" s="98"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="K37" s="90">
+        <v>15</v>
+      </c>
+      <c r="L37" s="90" t="s">
+        <v>192</v>
+      </c>
+      <c r="M37" s="103"/>
+      <c r="N37" s="98"/>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="90">
+        <v>16</v>
+      </c>
+      <c r="L38" s="90" t="s">
+        <v>193</v>
+      </c>
+      <c r="M38" s="104"/>
+      <c r="N38" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="N7:N22"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N23:N38"/>
+    <mergeCell ref="H23:H38"/>
+    <mergeCell ref="M23:M30"/>
+    <mergeCell ref="M31:M38"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="H7:H22"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M7:M14"/>
+    <mergeCell ref="M15:M22"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:S34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,22 +3745,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="66"/>
       <c r="J1" s="67"/>
-      <c r="P1" s="73" t="s">
+      <c r="P1" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
     </row>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" s="37" t="s">
@@ -3090,27 +3913,27 @@
       </c>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="77"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="87"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="71" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="45" t="s">
@@ -3119,19 +3942,19 @@
       <c r="G9" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="J9" s="83" t="s">
+      <c r="J9" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="85" t="s">
+      <c r="K9" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="L9" s="86" t="s">
+      <c r="L9" s="74" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3264,12 +4087,12 @@
       <c r="J15" s="50"/>
       <c r="K15" s="51"/>
       <c r="L15" s="51"/>
-      <c r="P15" s="78" t="s">
+      <c r="P15" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="88"/>
+      <c r="S15" s="88"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="24">
@@ -3290,7 +4113,7 @@
       <c r="J16" s="48"/>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
-      <c r="P16" s="82" t="s">
+      <c r="P16" s="70" t="s">
         <v>156</v>
       </c>
       <c r="Q16" s="43" t="s">
@@ -3315,19 +4138,18 @@
       </c>
       <c r="F17" s="48"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="87">
-        <v>2</v>
+      <c r="H17" s="75" t="s">
+        <v>161</v>
       </c>
       <c r="J17" s="48"/>
       <c r="K17" s="33"/>
-      <c r="L17" s="79">
-        <v>1</v>
-      </c>
-      <c r="P17" s="80">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="50">
+      <c r="L17" s="69">
+        <v>1</v>
+      </c>
+      <c r="P17" s="76">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="75">
         <v>1</v>
       </c>
       <c r="R17" s="50" t="s">
@@ -3356,10 +4178,10 @@
         <v>152</v>
       </c>
       <c r="L18" s="33"/>
-      <c r="P18" s="81">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="88">
+      <c r="P18" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="48">
         <v>2</v>
       </c>
       <c r="R18" s="48" t="s">
@@ -3384,10 +4206,10 @@
       </c>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
-      <c r="P19" s="81">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="48">
+      <c r="P19" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="75">
         <v>3</v>
       </c>
       <c r="R19" s="48" t="s">
@@ -3466,8 +4288,12 @@
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="D26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
@@ -3479,8 +4305,12 @@
       </c>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="D27" s="89">
+        <v>1</v>
+      </c>
+      <c r="E27" s="18">
+        <v>1</v>
+      </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
@@ -3492,6 +4322,12 @@
       </c>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
       <c r="M28" t="s">
         <v>140</v>
       </c>
@@ -3500,25 +4336,61 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="89">
+        <v>1</v>
+      </c>
+      <c r="E30" s="18">
+        <v>4</v>
+      </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="D31" s="18">
+        <v>2</v>
+      </c>
+      <c r="E31" s="18">
+        <v>1</v>
+      </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="D32" s="18">
+        <v>2</v>
+      </c>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="18">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="18">
+        <v>2</v>
+      </c>
+      <c r="E34" s="18">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>